<commit_message>
Cart count and clean cart codes added
</commit_message>
<xml_diff>
--- a/Excel Sheet/Order ID Creation Test Data.xlsx
+++ b/Excel Sheet/Order ID Creation Test Data.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Username</t>
   </si>
@@ -115,6 +115,12 @@
   </si>
   <si>
     <t>603424</t>
+  </si>
+  <si>
+    <t>201310</t>
+  </si>
+  <si>
+    <t>420565</t>
   </si>
 </sst>
 </file>
@@ -599,7 +605,7 @@
         <v>111</v>
       </c>
       <c r="N2" t="s" s="0">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>